<commit_message>
Updated RB Tier 2&3 Point Logic
</commit_message>
<xml_diff>
--- a/Files/ProgRegLogicCheck.xlsx
+++ b/Files/ProgRegLogicCheck.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40f61192ff96ff75/Documents/Git/madden22stats/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{CE9546DD-7D49-8243-AB22-42BE21F3C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB5FA70C-A892-418E-BCE3-66FEF0CCE830}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="13_ncr:1_{CE9546DD-7D49-8243-AB22-42BE21F3C011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{370B6764-15D3-43B1-9D17-AD02F2932AE4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09D5C185-7BCF-4CF5-9E1E-732FFFCB4F05}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{09D5C185-7BCF-4CF5-9E1E-732FFFCB4F05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9029" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9031" uniqueCount="215">
   <si>
     <t>StatCheck</t>
   </si>
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B87A0C8-4D85-4510-8C6C-E2406DAD465B}">
   <dimension ref="A1:H1765"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G195" sqref="G195"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1139,7 +1139,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1348,8 +1348,8 @@
       <c r="E14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="1">
-        <v>1</v>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -1726,8 +1726,8 @@
       <c r="E32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="1">
-        <v>1</v>
+      <c r="F32" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -1916,7 +1916,7 @@
         <v>7</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H41" s="1"/>
     </row>
@@ -1937,7 +1937,7 @@
         <v>8</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H42" s="1"/>
     </row>
@@ -1958,7 +1958,7 @@
         <v>9</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -2105,7 +2105,7 @@
         <v>3</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H50" s="1"/>
     </row>
@@ -2483,7 +2483,7 @@
         <v>3</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H68" s="1"/>
     </row>
@@ -2672,7 +2672,7 @@
         <v>7</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H77" s="1"/>
     </row>

</xml_diff>